<commit_message>
Upload tif (still wrong tho)
</commit_message>
<xml_diff>
--- a/doc/theory_pics/Figure 1.xlsx
+++ b/doc/theory_pics/Figure 1.xlsx
@@ -40,11 +40,14 @@
     <t>export_preset</t>
   </si>
   <si>
+    <t>export_path</t>
+  </si>
+  <si>
     <t>&lt;?xml version="1.0" encoding="utf-16"?&gt;_x000D_
 &lt;Preset xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance"&gt;_x000D_
-  &lt;Name&gt;Png, 500 dpi, RGB, Transparent canvas&lt;/Name&gt;_x000D_
-  &lt;Dpi&gt;500&lt;/Dpi&gt;_x000D_
-  &lt;FileType&gt;Png&lt;/FileType&gt;_x000D_
+  &lt;Name&gt;Emf&lt;/Name&gt;_x000D_
+  &lt;Dpi&gt;800&lt;/Dpi&gt;_x000D_
+  &lt;FileType&gt;Emf&lt;/FileType&gt;_x000D_
   &lt;ColorSpace&gt;Rgb&lt;/ColorSpace&gt;_x000D_
   &lt;Transparency&gt;TransparentCanvas&lt;/Transparency&gt;_x000D_
   &lt;UseColorProfile&gt;false&lt;/UseColorProfile&gt;_x000D_
@@ -52,10 +55,7 @@
 &lt;/Preset&gt;</t>
   </si>
   <si>
-    <t>export_path</t>
-  </si>
-  <si>
-    <t>C:\Users\liu.6544\Documents\GitHub\transfer\doc\theory_pics\picture_1_raw.png</t>
+    <t>C:\Users\liu.6544\Documents\GitHub\transfer\pic\figure_1.emf</t>
   </si>
 </sst>
 </file>
@@ -687,7 +687,7 @@
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -1378,13 +1378,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>65484</xdr:colOff>
+      <xdr:colOff>65483</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>602705</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>219807</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>115001</xdr:rowOff>
     </xdr:to>
@@ -1395,8 +1395,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11727656" y="5143500"/>
-          <a:ext cx="1144440" cy="305501"/>
+          <a:off x="11744598" y="5143500"/>
+          <a:ext cx="1370594" cy="305501"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1472,14 +1472,20 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1200"/>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
+            </a:rPr>
             <a:t>Receiving</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
+            </a:rPr>
             <a:t> stop</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200"/>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1671,146 +1677,55 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>113109</xdr:colOff>
+      <xdr:colOff>157071</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>126389</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>606504</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>42331</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>59714</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="9" name="Text Box 1"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="11775281" y="2405062"/>
-              <a:ext cx="493395" cy="314325"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr wrap="square" rtlCol="0">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr marL="0" marR="0">
-                <a:spcBef>
-                  <a:spcPts val="0"/>
-                </a:spcBef>
-                <a:spcAft>
-                  <a:spcPts val="0"/>
-                </a:spcAft>
-              </a:pPr>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1200" i="1">
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-                            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1200" i="1">
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-                            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑑</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1200" i="1">
-                            <a:effectLst/>
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-                            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑟</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1200">
-                <a:effectLst/>
-                <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
-                <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="9" name="Text Box 1"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="11775281" y="2405062"/>
-              <a:ext cx="493395" cy="314325"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr wrap="square" rtlCol="0">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr marL="0" marR="0">
-                <a:spcBef>
-                  <a:spcPts val="0"/>
-                </a:spcBef>
-                <a:spcAft>
-                  <a:spcPts val="0"/>
-                </a:spcAft>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" i="0">
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑑_𝑟</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1200">
-                <a:effectLst/>
-                <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
-                <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Text Box 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11836186" y="2412389"/>
+          <a:ext cx="493395" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:effectLst/>
+              <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
+              <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
+            </a:rPr>
+            <a:t>dr</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -1826,268 +1741,27 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>55959</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="10" name="Text Box 1"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="11755040" y="3170634"/>
-              <a:ext cx="493395" cy="314325"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr wrap="square" rtlCol="0">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr marL="0" marR="0">
-                <a:spcBef>
-                  <a:spcPts val="0"/>
-                </a:spcBef>
-                <a:spcAft>
-                  <a:spcPts val="0"/>
-                </a:spcAft>
-              </a:pPr>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1200" b="0" i="1">
-                        <a:effectLst/>
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-                        <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>𝐴𝑇𝑃</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1200">
-                <a:effectLst/>
-                <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
-                <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="10" name="Text Box 1"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="11755040" y="3170634"/>
-              <a:ext cx="493395" cy="314325"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr wrap="square" rtlCol="0">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr marL="0" marR="0">
-                <a:spcBef>
-                  <a:spcPts val="0"/>
-                </a:spcBef>
-                <a:spcAft>
-                  <a:spcPts val="0"/>
-                </a:spcAft>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0">
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝐴𝑇𝑃</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1200">
-                <a:effectLst/>
-                <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
-                <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>190976</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="Text Box 1"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="12574190" y="2900362"/>
-              <a:ext cx="493395" cy="314325"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr wrap="square" rtlCol="0">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr marL="0" marR="0">
-                <a:spcBef>
-                  <a:spcPts val="0"/>
-                </a:spcBef>
-                <a:spcAft>
-                  <a:spcPts val="0"/>
-                </a:spcAft>
-              </a:pPr>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1200" b="0" i="1">
-                        <a:effectLst/>
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-                        <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>𝑇𝑇𝑃</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1200">
-                <a:effectLst/>
-                <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
-                <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="11" name="Text Box 1"/>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="12574190" y="2900362"/>
-              <a:ext cx="493395" cy="314325"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr wrap="square" rtlCol="0">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr marL="0" marR="0">
-                <a:spcBef>
-                  <a:spcPts val="0"/>
-                </a:spcBef>
-                <a:spcAft>
-                  <a:spcPts val="0"/>
-                </a:spcAft>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0">
-                  <a:effectLst/>
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑇𝑇𝑃</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1200">
-                <a:effectLst/>
-                <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
-                <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-              </a:endParaRPr>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.26904</cdr:x>
-      <cdr:y>0.75485</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.4338</cdr:x>
-      <cdr:y>0.81561</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="Text Box 1"/>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2224360" y="3603201"/>
-          <a:ext cx="1362168" cy="290028"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Text Box 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11755040" y="3170634"/>
+          <a:ext cx="493395" cy="314325"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0">
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
           <a:noAutofit/>
         </a:bodyPr>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr marL="0" marR="0" algn="ctr">
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0">
             <a:spcBef>
               <a:spcPts val="0"/>
             </a:spcBef>
@@ -2098,39 +1772,197 @@
           <a:r>
             <a:rPr lang="en-US" sz="1200">
               <a:effectLst/>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
               <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>Generating</a:t>
+            <a:t>ATP</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1050">
-              <a:effectLst/>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>356087</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>242264</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Text Box 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12643337" y="2900362"/>
+          <a:ext cx="494312" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0">
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1200">
               <a:effectLst/>
-              <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
               <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>stop</a:t>
+            <a:t>TTP</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>540267</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>181708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>86457</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>106209</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Text Box 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9178709" y="5134708"/>
+          <a:ext cx="1370594" cy="305501"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0"/>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
+            </a:rPr>
+            <a:t>G</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1200">
+              <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
+            </a:rPr>
+            <a:t>enerating</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
+            </a:rPr>
+            <a:t> stop</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200">
-            <a:effectLst/>
-            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            <a:ea typeface="DengXian" panose="02010600030101010101" pitchFamily="2" charset="-122"/>
+            <a:latin typeface="SansSerif" panose="00000400000000000000" pitchFamily="2" charset="2"/>
           </a:endParaRPr>
         </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0.36628</cdr:x>
@@ -2461,12 +2293,12 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -2482,7 +2314,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>